<commit_message>
updating hypothesis testing analysis
</commit_message>
<xml_diff>
--- a/Lifelong_Learning/continuado_figuras_merito.xlsx
+++ b/Lifelong_Learning/continuado_figuras_merito.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/regina_costa_petrobras_com_br/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03812BCD-6381-4641-9FB3-083FE539FC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{657A7A9B-0309-45CD-82A9-49A8BA527A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6B0CA062-4A27-4625-BACC-90E1E58040B9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{6B0CA062-4A27-4625-BACC-90E1E58040B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Real" sheetId="2" r:id="rId1"/>
     <sheet name="WGAN_soFC" sheetId="3" r:id="rId2"/>
-    <sheet name="P2P_soFC" sheetId="5" r:id="rId3"/>
-    <sheet name="P2P_allshared" sheetId="6" r:id="rId4"/>
+    <sheet name="WGAN_allshared" sheetId="7" r:id="rId3"/>
+    <sheet name="P2P_soFC" sheetId="5" r:id="rId4"/>
+    <sheet name="P2P_allshared" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">P2P_allshared!$A$1:$A$91</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">P2P_soFC!$A$1:$P$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">P2P_allshared!$A$1:$A$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">P2P_soFC!$A$1:$P$91</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Real!$A$1:$P$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">WGAN_allshared!$A$1:$P$91</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">WGAN_soFC!$A$1:$P$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1774" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3230" uniqueCount="812">
   <si>
     <t>Sens TB Val</t>
   </si>
@@ -2160,6 +2162,327 @@
   </si>
   <si>
     <t>Shenzhenfinetune_best1_val2_test1_val2,pt</t>
+  </si>
+  <si>
+    <t>83.1</t>
+  </si>
+  <si>
+    <t>57.3</t>
+  </si>
+  <si>
+    <t>aux_test0_val2_test0_val2.pt</t>
+  </si>
+  <si>
+    <t>74.8</t>
+  </si>
+  <si>
+    <t>Shenzhenfinetune_test0_val3.pt</t>
+  </si>
+  <si>
+    <t>99.6</t>
+  </si>
+  <si>
+    <t>98.7</t>
+  </si>
+  <si>
+    <t>97.9</t>
+  </si>
+  <si>
+    <t>73.6</t>
+  </si>
+  <si>
+    <t>68.3</t>
+  </si>
+  <si>
+    <t>77.1</t>
+  </si>
+  <si>
+    <t>68.1</t>
+  </si>
+  <si>
+    <t>38.8</t>
+  </si>
+  <si>
+    <t>64.7</t>
+  </si>
+  <si>
+    <t>39.6</t>
+  </si>
+  <si>
+    <t>65.1</t>
+  </si>
+  <si>
+    <t>39.9</t>
+  </si>
+  <si>
+    <t>70.3</t>
+  </si>
+  <si>
+    <t>81.1</t>
+  </si>
+  <si>
+    <t>93.5</t>
+  </si>
+  <si>
+    <t>50.4</t>
+  </si>
+  <si>
+    <t>67.4</t>
+  </si>
+  <si>
+    <t>68.6</t>
+  </si>
+  <si>
+    <t>48.8</t>
+  </si>
+  <si>
+    <t>69.0</t>
+  </si>
+  <si>
+    <t>66.8</t>
+  </si>
+  <si>
+    <t>44.0</t>
+  </si>
+  <si>
+    <t>67.1</t>
+  </si>
+  <si>
+    <t>67.7</t>
+  </si>
+  <si>
+    <t>aux_test2_val0_test2_val0.pt</t>
+  </si>
+  <si>
+    <t>61.5</t>
+  </si>
+  <si>
+    <t>62.9</t>
+  </si>
+  <si>
+    <t>49.2</t>
+  </si>
+  <si>
+    <t>68.7</t>
+  </si>
+  <si>
+    <t>50.2</t>
+  </si>
+  <si>
+    <t>50.9</t>
+  </si>
+  <si>
+    <t>76.4</t>
+  </si>
+  <si>
+    <t>55.9</t>
+  </si>
+  <si>
+    <t>56.0</t>
+  </si>
+  <si>
+    <t>72.2</t>
+  </si>
+  <si>
+    <t>77.4</t>
+  </si>
+  <si>
+    <t>31.0</t>
+  </si>
+  <si>
+    <t>59.7</t>
+  </si>
+  <si>
+    <t>31.7</t>
+  </si>
+  <si>
+    <t>32.2</t>
+  </si>
+  <si>
+    <t>85.5</t>
+  </si>
+  <si>
+    <t>aux_test3_val2_test3_val2.pt</t>
+  </si>
+  <si>
+    <t>50.8</t>
+  </si>
+  <si>
+    <t>68.5</t>
+  </si>
+  <si>
+    <t>93.1</t>
+  </si>
+  <si>
+    <t>67.6</t>
+  </si>
+  <si>
+    <t>56.7</t>
+  </si>
+  <si>
+    <t>98.5</t>
+  </si>
+  <si>
+    <t>97.7</t>
+  </si>
+  <si>
+    <t>55.5</t>
+  </si>
+  <si>
+    <t>28.1</t>
+  </si>
+  <si>
+    <t>57.2</t>
+  </si>
+  <si>
+    <t>18.8</t>
+  </si>
+  <si>
+    <t>19.8</t>
+  </si>
+  <si>
+    <t>42.3</t>
+  </si>
+  <si>
+    <t>97.3</t>
+  </si>
+  <si>
+    <t>19.0</t>
+  </si>
+  <si>
+    <t>46.8</t>
+  </si>
+  <si>
+    <t>60.8</t>
+  </si>
+  <si>
+    <t>76.3</t>
+  </si>
+  <si>
+    <t>40.0</t>
+  </si>
+  <si>
+    <t>41.6</t>
+  </si>
+  <si>
+    <t>64.8</t>
+  </si>
+  <si>
+    <t>41.4</t>
+  </si>
+  <si>
+    <t>58.7</t>
+  </si>
+  <si>
+    <t>95.1</t>
+  </si>
+  <si>
+    <t>63.9</t>
+  </si>
+  <si>
+    <t>21.2</t>
+  </si>
+  <si>
+    <t>50.7</t>
+  </si>
+  <si>
+    <t>98.9</t>
+  </si>
+  <si>
+    <t>50.3</t>
+  </si>
+  <si>
+    <t>98.3</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>40.9</t>
+  </si>
+  <si>
+    <t>18.1</t>
+  </si>
+  <si>
+    <t>55.2</t>
+  </si>
+  <si>
+    <t>70.5</t>
+  </si>
+  <si>
+    <t>67.3</t>
+  </si>
+  <si>
+    <t>66.6</t>
+  </si>
+  <si>
+    <t>aux_test6_val5_test6_val5.pt</t>
+  </si>
+  <si>
+    <t>73.9</t>
+  </si>
+  <si>
+    <t>85.2</t>
+  </si>
+  <si>
+    <t>66.3</t>
+  </si>
+  <si>
+    <t>78.0</t>
+  </si>
+  <si>
+    <t>31.8</t>
+  </si>
+  <si>
+    <t>33.7</t>
+  </si>
+  <si>
+    <t>33.1</t>
+  </si>
+  <si>
+    <t>69.5</t>
+  </si>
+  <si>
+    <t>56.1</t>
+  </si>
+  <si>
+    <t>25.7</t>
+  </si>
+  <si>
+    <t>26.2</t>
+  </si>
+  <si>
+    <t>26.4</t>
+  </si>
+  <si>
+    <t>55.0</t>
+  </si>
+  <si>
+    <t>50.6</t>
+  </si>
+  <si>
+    <t>35.1</t>
+  </si>
+  <si>
+    <t>36.5</t>
+  </si>
+  <si>
+    <t>63.2</t>
+  </si>
+  <si>
+    <t>74.7</t>
+  </si>
+  <si>
+    <t>Shenzhenfinetune_test2_val8_test2_val8.pt</t>
+  </si>
+  <si>
+    <t>Shenzhenfinetune_test3_val8_test3_val8.pt</t>
+  </si>
+  <si>
+    <t>Shenzhenfinetune_test6_val8_test6_val8.pt</t>
+  </si>
+  <si>
+    <t>Shenzhenfinetune_best7_val5_test7_val5.pt</t>
   </si>
 </sst>
 </file>
@@ -2513,7 +2836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40374073-EC20-42C6-BE24-BE5A3314EAC9}">
   <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -11651,6 +11974,4575 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35F80F3-DC97-4223-AF5E-5C8A1EBDC247}">
+  <dimension ref="A1:P91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" t="s">
+        <v>705</v>
+      </c>
+      <c r="P2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>706</v>
+      </c>
+      <c r="G3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" t="s">
+        <v>610</v>
+      </c>
+      <c r="I3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" t="s">
+        <v>123</v>
+      </c>
+      <c r="O3" t="s">
+        <v>671</v>
+      </c>
+      <c r="P3" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>707</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>194</v>
+      </c>
+      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" t="s">
+        <v>708</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>709</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" t="s">
+        <v>710</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" t="s">
+        <v>711</v>
+      </c>
+      <c r="I5" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" t="s">
+        <v>278</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" t="s">
+        <v>178</v>
+      </c>
+      <c r="N5" t="s">
+        <v>712</v>
+      </c>
+      <c r="O5" t="s">
+        <v>111</v>
+      </c>
+      <c r="P5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H6" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>278</v>
+      </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" t="s">
+        <v>211</v>
+      </c>
+      <c r="O6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" t="s">
+        <v>320</v>
+      </c>
+      <c r="J7" t="s">
+        <v>217</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>328</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" t="s">
+        <v>247</v>
+      </c>
+      <c r="F8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" t="s">
+        <v>196</v>
+      </c>
+      <c r="I8" t="s">
+        <v>143</v>
+      </c>
+      <c r="J8" t="s">
+        <v>103</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" t="s">
+        <v>73</v>
+      </c>
+      <c r="M8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N8" t="s">
+        <v>247</v>
+      </c>
+      <c r="O8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>329</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F9" t="s">
+        <v>304</v>
+      </c>
+      <c r="G9" t="s">
+        <v>233</v>
+      </c>
+      <c r="H9" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" t="s">
+        <v>714</v>
+      </c>
+      <c r="J9" t="s">
+        <v>201</v>
+      </c>
+      <c r="K9" t="s">
+        <v>112</v>
+      </c>
+      <c r="L9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" t="s">
+        <v>715</v>
+      </c>
+      <c r="N9" t="s">
+        <v>293</v>
+      </c>
+      <c r="O9" t="s">
+        <v>716</v>
+      </c>
+      <c r="P9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>232</v>
+      </c>
+      <c r="F10" t="s">
+        <v>332</v>
+      </c>
+      <c r="G10" t="s">
+        <v>275</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>128</v>
+      </c>
+      <c r="J10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" t="s">
+        <v>167</v>
+      </c>
+      <c r="N10" t="s">
+        <v>182</v>
+      </c>
+      <c r="O10" t="s">
+        <v>71</v>
+      </c>
+      <c r="P10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" t="s">
+        <v>307</v>
+      </c>
+      <c r="H11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s">
+        <v>220</v>
+      </c>
+      <c r="K11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" t="s">
+        <v>705</v>
+      </c>
+      <c r="N11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>334</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" t="s">
+        <v>271</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" t="s">
+        <v>717</v>
+      </c>
+      <c r="G12" t="s">
+        <v>718</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>719</v>
+      </c>
+      <c r="J12" t="s">
+        <v>720</v>
+      </c>
+      <c r="K12" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M12" t="s">
+        <v>268</v>
+      </c>
+      <c r="N12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" t="s">
+        <v>721</v>
+      </c>
+      <c r="P12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>613</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>290</v>
+      </c>
+      <c r="E13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" t="s">
+        <v>112</v>
+      </c>
+      <c r="L13" t="s">
+        <v>98</v>
+      </c>
+      <c r="M13" t="s">
+        <v>103</v>
+      </c>
+      <c r="N13" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13" t="s">
+        <v>177</v>
+      </c>
+      <c r="P13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>336</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>397</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>295</v>
+      </c>
+      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" t="s">
+        <v>722</v>
+      </c>
+      <c r="J14" t="s">
+        <v>185</v>
+      </c>
+      <c r="K14" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" t="s">
+        <v>59</v>
+      </c>
+      <c r="M14" t="s">
+        <v>723</v>
+      </c>
+      <c r="N14" t="s">
+        <v>724</v>
+      </c>
+      <c r="O14" t="s">
+        <v>626</v>
+      </c>
+      <c r="P14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" t="s">
+        <v>725</v>
+      </c>
+      <c r="G15" t="s">
+        <v>251</v>
+      </c>
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" t="s">
+        <v>225</v>
+      </c>
+      <c r="J15" t="s">
+        <v>726</v>
+      </c>
+      <c r="K15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L15" t="s">
+        <v>158</v>
+      </c>
+      <c r="M15" t="s">
+        <v>727</v>
+      </c>
+      <c r="N15" t="s">
+        <v>76</v>
+      </c>
+      <c r="O15" t="s">
+        <v>728</v>
+      </c>
+      <c r="P15" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>339</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>305</v>
+      </c>
+      <c r="G16" t="s">
+        <v>399</v>
+      </c>
+      <c r="H16" t="s">
+        <v>284</v>
+      </c>
+      <c r="I16" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" t="s">
+        <v>258</v>
+      </c>
+      <c r="K16" t="s">
+        <v>180</v>
+      </c>
+      <c r="L16" t="s">
+        <v>158</v>
+      </c>
+      <c r="M16" t="s">
+        <v>261</v>
+      </c>
+      <c r="N16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" t="s">
+        <v>305</v>
+      </c>
+      <c r="P16" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>341</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" t="s">
+        <v>141</v>
+      </c>
+      <c r="I17" t="s">
+        <v>241</v>
+      </c>
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" t="s">
+        <v>112</v>
+      </c>
+      <c r="L17" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" t="s">
+        <v>103</v>
+      </c>
+      <c r="N17" t="s">
+        <v>84</v>
+      </c>
+      <c r="O17" t="s">
+        <v>72</v>
+      </c>
+      <c r="P17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>343</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" t="s">
+        <v>729</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" t="s">
+        <v>616</v>
+      </c>
+      <c r="G18" t="s">
+        <v>730</v>
+      </c>
+      <c r="H18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" t="s">
+        <v>731</v>
+      </c>
+      <c r="J18" t="s">
+        <v>732</v>
+      </c>
+      <c r="K18" t="s">
+        <v>180</v>
+      </c>
+      <c r="L18" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" t="s">
+        <v>261</v>
+      </c>
+      <c r="N18" t="s">
+        <v>123</v>
+      </c>
+      <c r="O18" t="s">
+        <v>623</v>
+      </c>
+      <c r="P18" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>614</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" t="s">
+        <v>350</v>
+      </c>
+      <c r="G19" t="s">
+        <v>248</v>
+      </c>
+      <c r="H19" t="s">
+        <v>248</v>
+      </c>
+      <c r="I19" t="s">
+        <v>239</v>
+      </c>
+      <c r="J19" t="s">
+        <v>125</v>
+      </c>
+      <c r="K19" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" t="s">
+        <v>162</v>
+      </c>
+      <c r="O19" t="s">
+        <v>239</v>
+      </c>
+      <c r="P19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>734</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>342</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" t="s">
+        <v>324</v>
+      </c>
+      <c r="H20" t="s">
+        <v>172</v>
+      </c>
+      <c r="I20" t="s">
+        <v>169</v>
+      </c>
+      <c r="J20" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" t="s">
+        <v>86</v>
+      </c>
+      <c r="L20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" t="s">
+        <v>115</v>
+      </c>
+      <c r="N20" t="s">
+        <v>257</v>
+      </c>
+      <c r="O20" t="s">
+        <v>237</v>
+      </c>
+      <c r="P20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>344</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>735</v>
+      </c>
+      <c r="G21" t="s">
+        <v>302</v>
+      </c>
+      <c r="H21" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" t="s">
+        <v>423</v>
+      </c>
+      <c r="J21" t="s">
+        <v>713</v>
+      </c>
+      <c r="K21" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" t="s">
+        <v>716</v>
+      </c>
+      <c r="N21" t="s">
+        <v>181</v>
+      </c>
+      <c r="O21" t="s">
+        <v>736</v>
+      </c>
+      <c r="P21" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>345</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>348</v>
+      </c>
+      <c r="F22" t="s">
+        <v>737</v>
+      </c>
+      <c r="G22" t="s">
+        <v>738</v>
+      </c>
+      <c r="H22" t="s">
+        <v>213</v>
+      </c>
+      <c r="I22" t="s">
+        <v>739</v>
+      </c>
+      <c r="J22" t="s">
+        <v>187</v>
+      </c>
+      <c r="K22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" t="s">
+        <v>186</v>
+      </c>
+      <c r="M22" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" t="s">
+        <v>213</v>
+      </c>
+      <c r="O22" t="s">
+        <v>740</v>
+      </c>
+      <c r="P22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>346</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>172</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" t="s">
+        <v>178</v>
+      </c>
+      <c r="H23" t="s">
+        <v>175</v>
+      </c>
+      <c r="I23" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" t="s">
+        <v>86</v>
+      </c>
+      <c r="M23" t="s">
+        <v>115</v>
+      </c>
+      <c r="N23" t="s">
+        <v>257</v>
+      </c>
+      <c r="O23" t="s">
+        <v>741</v>
+      </c>
+      <c r="P23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>347</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24" t="s">
+        <v>73</v>
+      </c>
+      <c r="M24" t="s">
+        <v>67</v>
+      </c>
+      <c r="N24" t="s">
+        <v>90</v>
+      </c>
+      <c r="O24" t="s">
+        <v>249</v>
+      </c>
+      <c r="P24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>618</v>
+      </c>
+      <c r="B25" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>742</v>
+      </c>
+      <c r="G25" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" t="s">
+        <v>284</v>
+      </c>
+      <c r="I25" t="s">
+        <v>743</v>
+      </c>
+      <c r="J25" t="s">
+        <v>168</v>
+      </c>
+      <c r="K25" t="s">
+        <v>98</v>
+      </c>
+      <c r="L25" t="s">
+        <v>164</v>
+      </c>
+      <c r="M25" t="s">
+        <v>744</v>
+      </c>
+      <c r="N25" t="s">
+        <v>314</v>
+      </c>
+      <c r="O25" t="s">
+        <v>256</v>
+      </c>
+      <c r="P25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>349</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>144</v>
+      </c>
+      <c r="G26" t="s">
+        <v>745</v>
+      </c>
+      <c r="H26" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" t="s">
+        <v>246</v>
+      </c>
+      <c r="J26" t="s">
+        <v>332</v>
+      </c>
+      <c r="K26" t="s">
+        <v>45</v>
+      </c>
+      <c r="L26" t="s">
+        <v>15</v>
+      </c>
+      <c r="M26" t="s">
+        <v>191</v>
+      </c>
+      <c r="N26" t="s">
+        <v>227</v>
+      </c>
+      <c r="O26" t="s">
+        <v>713</v>
+      </c>
+      <c r="P26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>351</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>288</v>
+      </c>
+      <c r="D27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" t="s">
+        <v>242</v>
+      </c>
+      <c r="F27" t="s">
+        <v>746</v>
+      </c>
+      <c r="G27" t="s">
+        <v>747</v>
+      </c>
+      <c r="H27" t="s">
+        <v>119</v>
+      </c>
+      <c r="I27" t="s">
+        <v>748</v>
+      </c>
+      <c r="J27" t="s">
+        <v>280</v>
+      </c>
+      <c r="K27" t="s">
+        <v>15</v>
+      </c>
+      <c r="L27" t="s">
+        <v>244</v>
+      </c>
+      <c r="M27" t="s">
+        <v>205</v>
+      </c>
+      <c r="N27" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" t="s">
+        <v>749</v>
+      </c>
+      <c r="P27" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>808</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>182</v>
+      </c>
+      <c r="D28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" t="s">
+        <v>196</v>
+      </c>
+      <c r="J28" t="s">
+        <v>73</v>
+      </c>
+      <c r="K28" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" t="s">
+        <v>55</v>
+      </c>
+      <c r="M28" t="s">
+        <v>272</v>
+      </c>
+      <c r="N28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O28" t="s">
+        <v>76</v>
+      </c>
+      <c r="P28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>354</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
+        <v>631</v>
+      </c>
+      <c r="E29" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" t="s">
+        <v>366</v>
+      </c>
+      <c r="H29" t="s">
+        <v>750</v>
+      </c>
+      <c r="I29" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29" t="s">
+        <v>307</v>
+      </c>
+      <c r="K29" t="s">
+        <v>15</v>
+      </c>
+      <c r="L29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M29" t="s">
+        <v>69</v>
+      </c>
+      <c r="N29" t="s">
+        <v>241</v>
+      </c>
+      <c r="O29" t="s">
+        <v>28</v>
+      </c>
+      <c r="P29" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>357</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" t="s">
+        <v>358</v>
+      </c>
+      <c r="G30" t="s">
+        <v>239</v>
+      </c>
+      <c r="H30" t="s">
+        <v>153</v>
+      </c>
+      <c r="I30" t="s">
+        <v>261</v>
+      </c>
+      <c r="J30" t="s">
+        <v>239</v>
+      </c>
+      <c r="K30" t="s">
+        <v>55</v>
+      </c>
+      <c r="L30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M30" t="s">
+        <v>212</v>
+      </c>
+      <c r="N30" t="s">
+        <v>207</v>
+      </c>
+      <c r="O30" t="s">
+        <v>28</v>
+      </c>
+      <c r="P30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>751</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>752</v>
+      </c>
+      <c r="G31" t="s">
+        <v>235</v>
+      </c>
+      <c r="H31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" t="s">
+        <v>240</v>
+      </c>
+      <c r="J31" t="s">
+        <v>320</v>
+      </c>
+      <c r="K31" t="s">
+        <v>51</v>
+      </c>
+      <c r="L31" t="s">
+        <v>56</v>
+      </c>
+      <c r="M31" t="s">
+        <v>147</v>
+      </c>
+      <c r="N31" t="s">
+        <v>52</v>
+      </c>
+      <c r="O31" t="s">
+        <v>630</v>
+      </c>
+      <c r="P31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>360</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" t="s">
+        <v>216</v>
+      </c>
+      <c r="G32" t="s">
+        <v>231</v>
+      </c>
+      <c r="H32" t="s">
+        <v>290</v>
+      </c>
+      <c r="I32" t="s">
+        <v>124</v>
+      </c>
+      <c r="J32" t="s">
+        <v>236</v>
+      </c>
+      <c r="K32" t="s">
+        <v>15</v>
+      </c>
+      <c r="L32" t="s">
+        <v>45</v>
+      </c>
+      <c r="M32" t="s">
+        <v>191</v>
+      </c>
+      <c r="N32" t="s">
+        <v>163</v>
+      </c>
+      <c r="O32" t="s">
+        <v>626</v>
+      </c>
+      <c r="P32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>361</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>244</v>
+      </c>
+      <c r="D33" t="s">
+        <v>245</v>
+      </c>
+      <c r="E33" t="s">
+        <v>348</v>
+      </c>
+      <c r="F33" t="s">
+        <v>273</v>
+      </c>
+      <c r="G33" t="s">
+        <v>338</v>
+      </c>
+      <c r="H33" t="s">
+        <v>161</v>
+      </c>
+      <c r="I33" t="s">
+        <v>616</v>
+      </c>
+      <c r="J33" t="s">
+        <v>122</v>
+      </c>
+      <c r="K33" t="s">
+        <v>73</v>
+      </c>
+      <c r="L33" t="s">
+        <v>158</v>
+      </c>
+      <c r="M33" t="s">
+        <v>753</v>
+      </c>
+      <c r="N33" t="s">
+        <v>213</v>
+      </c>
+      <c r="O33" t="s">
+        <v>273</v>
+      </c>
+      <c r="P33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>363</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
+        <v>304</v>
+      </c>
+      <c r="G34" t="s">
+        <v>155</v>
+      </c>
+      <c r="H34" t="s">
+        <v>754</v>
+      </c>
+      <c r="I34" t="s">
+        <v>755</v>
+      </c>
+      <c r="J34" t="s">
+        <v>60</v>
+      </c>
+      <c r="K34" t="s">
+        <v>51</v>
+      </c>
+      <c r="L34" t="s">
+        <v>22</v>
+      </c>
+      <c r="M34" t="s">
+        <v>93</v>
+      </c>
+      <c r="N34" t="s">
+        <v>724</v>
+      </c>
+      <c r="O34" t="s">
+        <v>716</v>
+      </c>
+      <c r="P34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>364</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>200</v>
+      </c>
+      <c r="D35" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" t="s">
+        <v>745</v>
+      </c>
+      <c r="G35" t="s">
+        <v>155</v>
+      </c>
+      <c r="H35" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35" t="s">
+        <v>217</v>
+      </c>
+      <c r="K35" t="s">
+        <v>73</v>
+      </c>
+      <c r="L35" t="s">
+        <v>86</v>
+      </c>
+      <c r="M35" t="s">
+        <v>130</v>
+      </c>
+      <c r="N35" t="s">
+        <v>181</v>
+      </c>
+      <c r="O35" t="s">
+        <v>86</v>
+      </c>
+      <c r="P35" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>365</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" t="s">
+        <v>320</v>
+      </c>
+      <c r="G36" t="s">
+        <v>723</v>
+      </c>
+      <c r="H36" t="s">
+        <v>153</v>
+      </c>
+      <c r="I36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" t="s">
+        <v>185</v>
+      </c>
+      <c r="K36" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" t="s">
+        <v>45</v>
+      </c>
+      <c r="M36" t="s">
+        <v>191</v>
+      </c>
+      <c r="N36" t="s">
+        <v>156</v>
+      </c>
+      <c r="O36" t="s">
+        <v>320</v>
+      </c>
+      <c r="P36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>809</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" t="s">
+        <v>162</v>
+      </c>
+      <c r="H37" t="s">
+        <v>96</v>
+      </c>
+      <c r="I37" t="s">
+        <v>182</v>
+      </c>
+      <c r="J37" t="s">
+        <v>194</v>
+      </c>
+      <c r="K37" t="s">
+        <v>98</v>
+      </c>
+      <c r="L37" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" t="s">
+        <v>16</v>
+      </c>
+      <c r="N37" t="s">
+        <v>101</v>
+      </c>
+      <c r="O37" t="s">
+        <v>277</v>
+      </c>
+      <c r="P37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>622</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" t="s">
+        <v>312</v>
+      </c>
+      <c r="F38" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" t="s">
+        <v>311</v>
+      </c>
+      <c r="I38" t="s">
+        <v>309</v>
+      </c>
+      <c r="J38" t="s">
+        <v>65</v>
+      </c>
+      <c r="K38" t="s">
+        <v>55</v>
+      </c>
+      <c r="L38" t="s">
+        <v>56</v>
+      </c>
+      <c r="M38" t="s">
+        <v>57</v>
+      </c>
+      <c r="N38" t="s">
+        <v>70</v>
+      </c>
+      <c r="O38" t="s">
+        <v>736</v>
+      </c>
+      <c r="P38" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>367</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39" t="s">
+        <v>177</v>
+      </c>
+      <c r="F39" t="s">
+        <v>299</v>
+      </c>
+      <c r="G39" t="s">
+        <v>295</v>
+      </c>
+      <c r="H39" t="s">
+        <v>77</v>
+      </c>
+      <c r="I39" t="s">
+        <v>756</v>
+      </c>
+      <c r="J39" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" t="s">
+        <v>98</v>
+      </c>
+      <c r="L39" t="s">
+        <v>225</v>
+      </c>
+      <c r="M39" t="s">
+        <v>263</v>
+      </c>
+      <c r="N39" t="s">
+        <v>278</v>
+      </c>
+      <c r="O39" t="s">
+        <v>299</v>
+      </c>
+      <c r="P39" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>368</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>164</v>
+      </c>
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" t="s">
+        <v>757</v>
+      </c>
+      <c r="F40" t="s">
+        <v>171</v>
+      </c>
+      <c r="G40" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" t="s">
+        <v>758</v>
+      </c>
+      <c r="I40" t="s">
+        <v>756</v>
+      </c>
+      <c r="J40" t="s">
+        <v>86</v>
+      </c>
+      <c r="K40" t="s">
+        <v>15</v>
+      </c>
+      <c r="L40" t="s">
+        <v>121</v>
+      </c>
+      <c r="M40" t="s">
+        <v>157</v>
+      </c>
+      <c r="N40" t="s">
+        <v>51</v>
+      </c>
+      <c r="O40" t="s">
+        <v>759</v>
+      </c>
+      <c r="P40" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>370</v>
+      </c>
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" t="s">
+        <v>181</v>
+      </c>
+      <c r="G41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H41" t="s">
+        <v>35</v>
+      </c>
+      <c r="I41" t="s">
+        <v>34</v>
+      </c>
+      <c r="J41" t="s">
+        <v>324</v>
+      </c>
+      <c r="K41" t="s">
+        <v>16</v>
+      </c>
+      <c r="L41" t="s">
+        <v>98</v>
+      </c>
+      <c r="M41" t="s">
+        <v>23</v>
+      </c>
+      <c r="N41" t="s">
+        <v>77</v>
+      </c>
+      <c r="O41" t="s">
+        <v>66</v>
+      </c>
+      <c r="P41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>624</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" t="s">
+        <v>191</v>
+      </c>
+      <c r="G42" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" t="s">
+        <v>74</v>
+      </c>
+      <c r="I42" t="s">
+        <v>220</v>
+      </c>
+      <c r="J42" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42" t="s">
+        <v>16</v>
+      </c>
+      <c r="L42" t="s">
+        <v>16</v>
+      </c>
+      <c r="M42" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" t="s">
+        <v>196</v>
+      </c>
+      <c r="O42" t="s">
+        <v>155</v>
+      </c>
+      <c r="P42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>371</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" t="s">
+        <v>760</v>
+      </c>
+      <c r="D43" t="s">
+        <v>761</v>
+      </c>
+      <c r="E43" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" t="s">
+        <v>762</v>
+      </c>
+      <c r="G43" t="s">
+        <v>197</v>
+      </c>
+      <c r="H43" t="s">
+        <v>758</v>
+      </c>
+      <c r="I43" t="s">
+        <v>763</v>
+      </c>
+      <c r="J43" t="s">
+        <v>752</v>
+      </c>
+      <c r="K43" t="s">
+        <v>55</v>
+      </c>
+      <c r="L43" t="s">
+        <v>688</v>
+      </c>
+      <c r="M43" t="s">
+        <v>764</v>
+      </c>
+      <c r="N43" t="s">
+        <v>765</v>
+      </c>
+      <c r="O43" t="s">
+        <v>766</v>
+      </c>
+      <c r="P43" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>372</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" t="s">
+        <v>177</v>
+      </c>
+      <c r="E44" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G44" t="s">
+        <v>183</v>
+      </c>
+      <c r="H44" t="s">
+        <v>750</v>
+      </c>
+      <c r="I44" t="s">
+        <v>373</v>
+      </c>
+      <c r="J44" t="s">
+        <v>183</v>
+      </c>
+      <c r="K44" t="s">
+        <v>25</v>
+      </c>
+      <c r="L44" t="s">
+        <v>15</v>
+      </c>
+      <c r="M44" t="s">
+        <v>66</v>
+      </c>
+      <c r="N44" t="s">
+        <v>98</v>
+      </c>
+      <c r="O44" t="s">
+        <v>92</v>
+      </c>
+      <c r="P44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>374</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>286</v>
+      </c>
+      <c r="D45" t="s">
+        <v>338</v>
+      </c>
+      <c r="E45" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" t="s">
+        <v>664</v>
+      </c>
+      <c r="G45" t="s">
+        <v>362</v>
+      </c>
+      <c r="H45" t="s">
+        <v>284</v>
+      </c>
+      <c r="I45" t="s">
+        <v>767</v>
+      </c>
+      <c r="J45" t="s">
+        <v>729</v>
+      </c>
+      <c r="K45" t="s">
+        <v>55</v>
+      </c>
+      <c r="L45" t="s">
+        <v>190</v>
+      </c>
+      <c r="M45" t="s">
+        <v>747</v>
+      </c>
+      <c r="N45" t="s">
+        <v>123</v>
+      </c>
+      <c r="O45" t="s">
+        <v>265</v>
+      </c>
+      <c r="P45" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>375</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46" t="s">
+        <v>173</v>
+      </c>
+      <c r="G46" t="s">
+        <v>44</v>
+      </c>
+      <c r="H46" t="s">
+        <v>94</v>
+      </c>
+      <c r="I46" t="s">
+        <v>768</v>
+      </c>
+      <c r="J46" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" t="s">
+        <v>98</v>
+      </c>
+      <c r="L46" t="s">
+        <v>164</v>
+      </c>
+      <c r="M46" t="s">
+        <v>744</v>
+      </c>
+      <c r="N46" t="s">
+        <v>84</v>
+      </c>
+      <c r="O46" t="s">
+        <v>137</v>
+      </c>
+      <c r="P46" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>376</v>
+      </c>
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" t="s">
+        <v>753</v>
+      </c>
+      <c r="G47" t="s">
+        <v>666</v>
+      </c>
+      <c r="H47" t="s">
+        <v>142</v>
+      </c>
+      <c r="I47" t="s">
+        <v>216</v>
+      </c>
+      <c r="J47" t="s">
+        <v>222</v>
+      </c>
+      <c r="K47" t="s">
+        <v>98</v>
+      </c>
+      <c r="L47" t="s">
+        <v>186</v>
+      </c>
+      <c r="M47" t="s">
+        <v>129</v>
+      </c>
+      <c r="N47" t="s">
+        <v>142</v>
+      </c>
+      <c r="O47" t="s">
+        <v>251</v>
+      </c>
+      <c r="P47" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>377</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" t="s">
+        <v>166</v>
+      </c>
+      <c r="G48" t="s">
+        <v>64</v>
+      </c>
+      <c r="H48" t="s">
+        <v>278</v>
+      </c>
+      <c r="I48" t="s">
+        <v>146</v>
+      </c>
+      <c r="J48" t="s">
+        <v>307</v>
+      </c>
+      <c r="K48" t="s">
+        <v>15</v>
+      </c>
+      <c r="L48" t="s">
+        <v>45</v>
+      </c>
+      <c r="M48" t="s">
+        <v>191</v>
+      </c>
+      <c r="N48" t="s">
+        <v>77</v>
+      </c>
+      <c r="O48" t="s">
+        <v>166</v>
+      </c>
+      <c r="P48" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>382</v>
+      </c>
+      <c r="B49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" t="s">
+        <v>770</v>
+      </c>
+      <c r="G49" t="s">
+        <v>309</v>
+      </c>
+      <c r="H49" t="s">
+        <v>754</v>
+      </c>
+      <c r="I49" t="s">
+        <v>771</v>
+      </c>
+      <c r="J49" t="s">
+        <v>772</v>
+      </c>
+      <c r="K49" t="s">
+        <v>15</v>
+      </c>
+      <c r="L49" t="s">
+        <v>269</v>
+      </c>
+      <c r="M49" t="s">
+        <v>270</v>
+      </c>
+      <c r="N49" t="s">
+        <v>293</v>
+      </c>
+      <c r="O49" t="s">
+        <v>773</v>
+      </c>
+      <c r="P49" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>628</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" t="s">
+        <v>212</v>
+      </c>
+      <c r="E50" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" t="s">
+        <v>716</v>
+      </c>
+      <c r="G50" t="s">
+        <v>130</v>
+      </c>
+      <c r="H50" t="s">
+        <v>52</v>
+      </c>
+      <c r="I50" t="s">
+        <v>714</v>
+      </c>
+      <c r="J50" t="s">
+        <v>130</v>
+      </c>
+      <c r="K50" t="s">
+        <v>51</v>
+      </c>
+      <c r="L50" t="s">
+        <v>56</v>
+      </c>
+      <c r="M50" t="s">
+        <v>147</v>
+      </c>
+      <c r="N50" t="s">
+        <v>52</v>
+      </c>
+      <c r="O50" t="s">
+        <v>268</v>
+      </c>
+      <c r="P50" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>385</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" t="s">
+        <v>191</v>
+      </c>
+      <c r="E51" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" t="s">
+        <v>86</v>
+      </c>
+      <c r="G51" t="s">
+        <v>38</v>
+      </c>
+      <c r="H51" t="s">
+        <v>290</v>
+      </c>
+      <c r="I51" t="s">
+        <v>170</v>
+      </c>
+      <c r="J51" t="s">
+        <v>194</v>
+      </c>
+      <c r="K51" t="s">
+        <v>51</v>
+      </c>
+      <c r="L51" t="s">
+        <v>164</v>
+      </c>
+      <c r="M51" t="s">
+        <v>165</v>
+      </c>
+      <c r="N51" t="s">
+        <v>293</v>
+      </c>
+      <c r="O51" t="s">
+        <v>713</v>
+      </c>
+      <c r="P51" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>629</v>
+      </c>
+      <c r="B52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" t="s">
+        <v>182</v>
+      </c>
+      <c r="E52" t="s">
+        <v>139</v>
+      </c>
+      <c r="F52" t="s">
+        <v>705</v>
+      </c>
+      <c r="G52" t="s">
+        <v>409</v>
+      </c>
+      <c r="H52" t="s">
+        <v>96</v>
+      </c>
+      <c r="I52" t="s">
+        <v>239</v>
+      </c>
+      <c r="J52" t="s">
+        <v>31</v>
+      </c>
+      <c r="K52" t="s">
+        <v>15</v>
+      </c>
+      <c r="L52" t="s">
+        <v>25</v>
+      </c>
+      <c r="M52" t="s">
+        <v>66</v>
+      </c>
+      <c r="N52" t="s">
+        <v>17</v>
+      </c>
+      <c r="O52" t="s">
+        <v>69</v>
+      </c>
+      <c r="P52" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>388</v>
+      </c>
+      <c r="B53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" t="s">
+        <v>182</v>
+      </c>
+      <c r="E53" t="s">
+        <v>275</v>
+      </c>
+      <c r="F53" t="s">
+        <v>194</v>
+      </c>
+      <c r="G53" t="s">
+        <v>185</v>
+      </c>
+      <c r="H53" t="s">
+        <v>169</v>
+      </c>
+      <c r="I53" t="s">
+        <v>125</v>
+      </c>
+      <c r="J53" t="s">
+        <v>212</v>
+      </c>
+      <c r="K53" t="s">
+        <v>98</v>
+      </c>
+      <c r="L53" t="s">
+        <v>45</v>
+      </c>
+      <c r="M53" t="s">
+        <v>715</v>
+      </c>
+      <c r="N53" t="s">
+        <v>277</v>
+      </c>
+      <c r="O53" t="s">
+        <v>277</v>
+      </c>
+      <c r="P53" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>389</v>
+      </c>
+      <c r="B54" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" t="s">
+        <v>671</v>
+      </c>
+      <c r="G54" t="s">
+        <v>260</v>
+      </c>
+      <c r="H54" t="s">
+        <v>161</v>
+      </c>
+      <c r="I54" t="s">
+        <v>774</v>
+      </c>
+      <c r="J54" t="s">
+        <v>260</v>
+      </c>
+      <c r="K54" t="s">
+        <v>51</v>
+      </c>
+      <c r="L54" t="s">
+        <v>56</v>
+      </c>
+      <c r="M54" t="s">
+        <v>147</v>
+      </c>
+      <c r="N54" t="s">
+        <v>163</v>
+      </c>
+      <c r="O54" t="s">
+        <v>416</v>
+      </c>
+      <c r="P54" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>390</v>
+      </c>
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F55" t="s">
+        <v>66</v>
+      </c>
+      <c r="G55" t="s">
+        <v>66</v>
+      </c>
+      <c r="H55" t="s">
+        <v>750</v>
+      </c>
+      <c r="I55" t="s">
+        <v>162</v>
+      </c>
+      <c r="J55" t="s">
+        <v>142</v>
+      </c>
+      <c r="K55" t="s">
+        <v>98</v>
+      </c>
+      <c r="L55" t="s">
+        <v>25</v>
+      </c>
+      <c r="M55" t="s">
+        <v>16</v>
+      </c>
+      <c r="N55" t="s">
+        <v>89</v>
+      </c>
+      <c r="O55" t="s">
+        <v>705</v>
+      </c>
+      <c r="P55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>391</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" t="s">
+        <v>775</v>
+      </c>
+      <c r="F56" t="s">
+        <v>200</v>
+      </c>
+      <c r="G56" t="s">
+        <v>71</v>
+      </c>
+      <c r="H56" t="s">
+        <v>21</v>
+      </c>
+      <c r="I56" t="s">
+        <v>776</v>
+      </c>
+      <c r="J56" t="s">
+        <v>223</v>
+      </c>
+      <c r="K56" t="s">
+        <v>39</v>
+      </c>
+      <c r="L56" t="s">
+        <v>200</v>
+      </c>
+      <c r="M56" t="s">
+        <v>176</v>
+      </c>
+      <c r="N56" t="s">
+        <v>70</v>
+      </c>
+      <c r="O56" t="s">
+        <v>309</v>
+      </c>
+      <c r="P56" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>392</v>
+      </c>
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" t="s">
+        <v>178</v>
+      </c>
+      <c r="E57" t="s">
+        <v>95</v>
+      </c>
+      <c r="F57" t="s">
+        <v>169</v>
+      </c>
+      <c r="G57" t="s">
+        <v>98</v>
+      </c>
+      <c r="H57" t="s">
+        <v>74</v>
+      </c>
+      <c r="I57" t="s">
+        <v>201</v>
+      </c>
+      <c r="J57" t="s">
+        <v>98</v>
+      </c>
+      <c r="K57" t="s">
+        <v>39</v>
+      </c>
+      <c r="L57" t="s">
+        <v>82</v>
+      </c>
+      <c r="M57" t="s">
+        <v>182</v>
+      </c>
+      <c r="N57" t="s">
+        <v>87</v>
+      </c>
+      <c r="O57" t="s">
+        <v>292</v>
+      </c>
+      <c r="P57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>393</v>
+      </c>
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
+        <v>777</v>
+      </c>
+      <c r="D58" t="s">
+        <v>778</v>
+      </c>
+      <c r="E58" t="s">
+        <v>779</v>
+      </c>
+      <c r="F58" t="s">
+        <v>762</v>
+      </c>
+      <c r="G58" t="s">
+        <v>780</v>
+      </c>
+      <c r="H58" t="s">
+        <v>781</v>
+      </c>
+      <c r="I58" t="s">
+        <v>766</v>
+      </c>
+      <c r="J58" t="s">
+        <v>725</v>
+      </c>
+      <c r="K58" t="s">
+        <v>180</v>
+      </c>
+      <c r="L58" t="s">
+        <v>782</v>
+      </c>
+      <c r="M58" t="s">
+        <v>783</v>
+      </c>
+      <c r="N58" t="s">
+        <v>757</v>
+      </c>
+      <c r="O58" t="s">
+        <v>784</v>
+      </c>
+      <c r="P58" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>395</v>
+      </c>
+      <c r="B59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" t="s">
+        <v>225</v>
+      </c>
+      <c r="D59" t="s">
+        <v>209</v>
+      </c>
+      <c r="E59" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" t="s">
+        <v>785</v>
+      </c>
+      <c r="G59" t="s">
+        <v>230</v>
+      </c>
+      <c r="H59" t="s">
+        <v>79</v>
+      </c>
+      <c r="I59" t="s">
+        <v>697</v>
+      </c>
+      <c r="J59" t="s">
+        <v>611</v>
+      </c>
+      <c r="K59" t="s">
+        <v>292</v>
+      </c>
+      <c r="L59" t="s">
+        <v>133</v>
+      </c>
+      <c r="M59" t="s">
+        <v>729</v>
+      </c>
+      <c r="N59" t="s">
+        <v>77</v>
+      </c>
+      <c r="O59" t="s">
+        <v>188</v>
+      </c>
+      <c r="P59" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>396</v>
+      </c>
+      <c r="B60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" t="s">
+        <v>45</v>
+      </c>
+      <c r="D60" t="s">
+        <v>191</v>
+      </c>
+      <c r="E60" t="s">
+        <v>311</v>
+      </c>
+      <c r="F60" t="s">
+        <v>381</v>
+      </c>
+      <c r="G60" t="s">
+        <v>233</v>
+      </c>
+      <c r="H60" t="s">
+        <v>47</v>
+      </c>
+      <c r="I60" t="s">
+        <v>787</v>
+      </c>
+      <c r="J60" t="s">
+        <v>155</v>
+      </c>
+      <c r="K60" t="s">
+        <v>112</v>
+      </c>
+      <c r="L60" t="s">
+        <v>133</v>
+      </c>
+      <c r="M60" t="s">
+        <v>135</v>
+      </c>
+      <c r="N60" t="s">
+        <v>724</v>
+      </c>
+      <c r="O60" t="s">
+        <v>788</v>
+      </c>
+      <c r="P60" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>789</v>
+      </c>
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" t="s">
+        <v>66</v>
+      </c>
+      <c r="E61" t="s">
+        <v>160</v>
+      </c>
+      <c r="F61" t="s">
+        <v>155</v>
+      </c>
+      <c r="G61" t="s">
+        <v>96</v>
+      </c>
+      <c r="H61" t="s">
+        <v>161</v>
+      </c>
+      <c r="I61" t="s">
+        <v>220</v>
+      </c>
+      <c r="J61" t="s">
+        <v>101</v>
+      </c>
+      <c r="K61" t="s">
+        <v>39</v>
+      </c>
+      <c r="L61" t="s">
+        <v>131</v>
+      </c>
+      <c r="M61" t="s">
+        <v>132</v>
+      </c>
+      <c r="N61" t="s">
+        <v>161</v>
+      </c>
+      <c r="O61" t="s">
+        <v>25</v>
+      </c>
+      <c r="P61" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>398</v>
+      </c>
+      <c r="B62" t="s">
+        <v>39</v>
+      </c>
+      <c r="C62" t="s">
+        <v>91</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" t="s">
+        <v>167</v>
+      </c>
+      <c r="F62" t="s">
+        <v>233</v>
+      </c>
+      <c r="G62" t="s">
+        <v>132</v>
+      </c>
+      <c r="H62" t="s">
+        <v>169</v>
+      </c>
+      <c r="I62" t="s">
+        <v>132</v>
+      </c>
+      <c r="J62" t="s">
+        <v>191</v>
+      </c>
+      <c r="K62" t="s">
+        <v>129</v>
+      </c>
+      <c r="L62" t="s">
+        <v>131</v>
+      </c>
+      <c r="M62" t="s">
+        <v>45</v>
+      </c>
+      <c r="N62" t="s">
+        <v>310</v>
+      </c>
+      <c r="O62" t="s">
+        <v>67</v>
+      </c>
+      <c r="P62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>400</v>
+      </c>
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" t="s">
+        <v>182</v>
+      </c>
+      <c r="E63" t="s">
+        <v>204</v>
+      </c>
+      <c r="F63" t="s">
+        <v>46</v>
+      </c>
+      <c r="G63" t="s">
+        <v>272</v>
+      </c>
+      <c r="H63" t="s">
+        <v>204</v>
+      </c>
+      <c r="I63" t="s">
+        <v>399</v>
+      </c>
+      <c r="J63" t="s">
+        <v>248</v>
+      </c>
+      <c r="K63" t="s">
+        <v>24</v>
+      </c>
+      <c r="L63" t="s">
+        <v>200</v>
+      </c>
+      <c r="M63" t="s">
+        <v>138</v>
+      </c>
+      <c r="N63" t="s">
+        <v>218</v>
+      </c>
+      <c r="O63" t="s">
+        <v>790</v>
+      </c>
+      <c r="P63" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>810</v>
+      </c>
+      <c r="B64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" t="s">
+        <v>184</v>
+      </c>
+      <c r="E64" t="s">
+        <v>204</v>
+      </c>
+      <c r="F64" t="s">
+        <v>130</v>
+      </c>
+      <c r="G64" t="s">
+        <v>106</v>
+      </c>
+      <c r="H64" t="s">
+        <v>211</v>
+      </c>
+      <c r="I64" t="s">
+        <v>232</v>
+      </c>
+      <c r="J64" t="s">
+        <v>96</v>
+      </c>
+      <c r="K64" t="s">
+        <v>39</v>
+      </c>
+      <c r="L64" t="s">
+        <v>131</v>
+      </c>
+      <c r="M64" t="s">
+        <v>132</v>
+      </c>
+      <c r="N64" t="s">
+        <v>211</v>
+      </c>
+      <c r="O64" t="s">
+        <v>292</v>
+      </c>
+      <c r="P64" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>402</v>
+      </c>
+      <c r="B65" t="s">
+        <v>39</v>
+      </c>
+      <c r="C65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65" t="s">
+        <v>40</v>
+      </c>
+      <c r="E65" t="s">
+        <v>204</v>
+      </c>
+      <c r="F65" t="s">
+        <v>792</v>
+      </c>
+      <c r="G65" t="s">
+        <v>793</v>
+      </c>
+      <c r="H65" t="s">
+        <v>204</v>
+      </c>
+      <c r="I65" t="s">
+        <v>209</v>
+      </c>
+      <c r="J65" t="s">
+        <v>64</v>
+      </c>
+      <c r="K65" t="s">
+        <v>36</v>
+      </c>
+      <c r="L65" t="s">
+        <v>286</v>
+      </c>
+      <c r="M65" t="s">
+        <v>330</v>
+      </c>
+      <c r="N65" t="s">
+        <v>211</v>
+      </c>
+      <c r="O65" t="s">
+        <v>122</v>
+      </c>
+      <c r="P65" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>403</v>
+      </c>
+      <c r="B66" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E66" t="s">
+        <v>68</v>
+      </c>
+      <c r="F66" t="s">
+        <v>67</v>
+      </c>
+      <c r="G66" t="s">
+        <v>238</v>
+      </c>
+      <c r="H66" t="s">
+        <v>94</v>
+      </c>
+      <c r="I66" t="s">
+        <v>61</v>
+      </c>
+      <c r="J66" t="s">
+        <v>20</v>
+      </c>
+      <c r="K66" t="s">
+        <v>112</v>
+      </c>
+      <c r="L66" t="s">
+        <v>171</v>
+      </c>
+      <c r="M66" t="s">
+        <v>146</v>
+      </c>
+      <c r="N66" t="s">
+        <v>85</v>
+      </c>
+      <c r="O66" t="s">
+        <v>50</v>
+      </c>
+      <c r="P66" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>404</v>
+      </c>
+      <c r="B67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" t="s">
+        <v>225</v>
+      </c>
+      <c r="D67" t="s">
+        <v>209</v>
+      </c>
+      <c r="E67" t="s">
+        <v>311</v>
+      </c>
+      <c r="F67" t="s">
+        <v>794</v>
+      </c>
+      <c r="G67" t="s">
+        <v>700</v>
+      </c>
+      <c r="H67" t="s">
+        <v>47</v>
+      </c>
+      <c r="I67" t="s">
+        <v>795</v>
+      </c>
+      <c r="J67" t="s">
+        <v>280</v>
+      </c>
+      <c r="K67" t="s">
+        <v>105</v>
+      </c>
+      <c r="L67" t="s">
+        <v>760</v>
+      </c>
+      <c r="M67" t="s">
+        <v>761</v>
+      </c>
+      <c r="N67" t="s">
+        <v>70</v>
+      </c>
+      <c r="O67" t="s">
+        <v>796</v>
+      </c>
+      <c r="P67" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>405</v>
+      </c>
+      <c r="B68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" t="s">
+        <v>59</v>
+      </c>
+      <c r="D68" t="s">
+        <v>397</v>
+      </c>
+      <c r="E68" t="s">
+        <v>30</v>
+      </c>
+      <c r="F68" t="s">
+        <v>59</v>
+      </c>
+      <c r="G68" t="s">
+        <v>292</v>
+      </c>
+      <c r="H68" t="s">
+        <v>33</v>
+      </c>
+      <c r="I68" t="s">
+        <v>59</v>
+      </c>
+      <c r="J68" t="s">
+        <v>307</v>
+      </c>
+      <c r="K68" t="s">
+        <v>36</v>
+      </c>
+      <c r="L68" t="s">
+        <v>197</v>
+      </c>
+      <c r="M68" t="s">
+        <v>722</v>
+      </c>
+      <c r="N68" t="s">
+        <v>37</v>
+      </c>
+      <c r="O68" t="s">
+        <v>120</v>
+      </c>
+      <c r="P68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>406</v>
+      </c>
+      <c r="B69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" t="s">
+        <v>59</v>
+      </c>
+      <c r="D69" t="s">
+        <v>397</v>
+      </c>
+      <c r="E69" t="s">
+        <v>36</v>
+      </c>
+      <c r="F69" t="s">
+        <v>772</v>
+      </c>
+      <c r="G69" t="s">
+        <v>195</v>
+      </c>
+      <c r="H69" t="s">
+        <v>172</v>
+      </c>
+      <c r="I69" t="s">
+        <v>120</v>
+      </c>
+      <c r="J69" t="s">
+        <v>195</v>
+      </c>
+      <c r="K69" t="s">
+        <v>105</v>
+      </c>
+      <c r="L69" t="s">
+        <v>197</v>
+      </c>
+      <c r="M69" t="s">
+        <v>144</v>
+      </c>
+      <c r="N69" t="s">
+        <v>47</v>
+      </c>
+      <c r="O69" t="s">
+        <v>110</v>
+      </c>
+      <c r="P69" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>811</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>98</v>
+      </c>
+      <c r="D70" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" t="s">
+        <v>72</v>
+      </c>
+      <c r="F70" t="s">
+        <v>207</v>
+      </c>
+      <c r="G70" t="s">
+        <v>80</v>
+      </c>
+      <c r="H70" t="s">
+        <v>40</v>
+      </c>
+      <c r="I70" t="s">
+        <v>229</v>
+      </c>
+      <c r="J70" t="s">
+        <v>80</v>
+      </c>
+      <c r="K70" t="s">
+        <v>39</v>
+      </c>
+      <c r="L70" t="s">
+        <v>210</v>
+      </c>
+      <c r="M70" t="s">
+        <v>15</v>
+      </c>
+      <c r="N70" t="s">
+        <v>84</v>
+      </c>
+      <c r="O70" t="s">
+        <v>218</v>
+      </c>
+      <c r="P70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>407</v>
+      </c>
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" t="s">
+        <v>150</v>
+      </c>
+      <c r="E71" t="s">
+        <v>160</v>
+      </c>
+      <c r="F71" t="s">
+        <v>797</v>
+      </c>
+      <c r="G71" t="s">
+        <v>233</v>
+      </c>
+      <c r="H71" t="s">
+        <v>161</v>
+      </c>
+      <c r="I71" t="s">
+        <v>251</v>
+      </c>
+      <c r="J71" t="s">
+        <v>132</v>
+      </c>
+      <c r="K71" t="s">
+        <v>36</v>
+      </c>
+      <c r="L71" t="s">
+        <v>197</v>
+      </c>
+      <c r="M71" t="s">
+        <v>722</v>
+      </c>
+      <c r="N71" t="s">
+        <v>257</v>
+      </c>
+      <c r="O71" t="s">
+        <v>788</v>
+      </c>
+      <c r="P71" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>639</v>
+      </c>
+      <c r="B72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72" t="s">
+        <v>200</v>
+      </c>
+      <c r="D72" t="s">
+        <v>176</v>
+      </c>
+      <c r="E72" t="s">
+        <v>316</v>
+      </c>
+      <c r="F72" t="s">
+        <v>798</v>
+      </c>
+      <c r="G72" t="s">
+        <v>159</v>
+      </c>
+      <c r="H72" t="s">
+        <v>211</v>
+      </c>
+      <c r="I72" t="s">
+        <v>296</v>
+      </c>
+      <c r="J72" t="s">
+        <v>57</v>
+      </c>
+      <c r="K72" t="s">
+        <v>36</v>
+      </c>
+      <c r="L72" t="s">
+        <v>294</v>
+      </c>
+      <c r="M72" t="s">
+        <v>205</v>
+      </c>
+      <c r="N72" t="s">
+        <v>213</v>
+      </c>
+      <c r="O72" t="s">
+        <v>53</v>
+      </c>
+      <c r="P72" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>408</v>
+      </c>
+      <c r="B73" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" t="s">
+        <v>210</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" t="s">
+        <v>279</v>
+      </c>
+      <c r="F73" t="s">
+        <v>724</v>
+      </c>
+      <c r="G73" t="s">
+        <v>93</v>
+      </c>
+      <c r="H73" t="s">
+        <v>128</v>
+      </c>
+      <c r="I73" t="s">
+        <v>37</v>
+      </c>
+      <c r="J73" t="s">
+        <v>791</v>
+      </c>
+      <c r="K73" t="s">
+        <v>112</v>
+      </c>
+      <c r="L73" t="s">
+        <v>27</v>
+      </c>
+      <c r="M73" t="s">
+        <v>316</v>
+      </c>
+      <c r="N73" t="s">
+        <v>223</v>
+      </c>
+      <c r="O73" t="s">
+        <v>30</v>
+      </c>
+      <c r="P73" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>410</v>
+      </c>
+      <c r="B74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" t="s">
+        <v>40</v>
+      </c>
+      <c r="E74" t="s">
+        <v>87</v>
+      </c>
+      <c r="F74" t="s">
+        <v>144</v>
+      </c>
+      <c r="G74" t="s">
+        <v>237</v>
+      </c>
+      <c r="H74" t="s">
+        <v>88</v>
+      </c>
+      <c r="I74" t="s">
+        <v>243</v>
+      </c>
+      <c r="J74" t="s">
+        <v>277</v>
+      </c>
+      <c r="K74" t="s">
+        <v>112</v>
+      </c>
+      <c r="L74" t="s">
+        <v>82</v>
+      </c>
+      <c r="M74" t="s">
+        <v>60</v>
+      </c>
+      <c r="N74" t="s">
+        <v>87</v>
+      </c>
+      <c r="O74" t="s">
+        <v>22</v>
+      </c>
+      <c r="P74" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>640</v>
+      </c>
+      <c r="B75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75" t="s">
+        <v>59</v>
+      </c>
+      <c r="D75" t="s">
+        <v>65</v>
+      </c>
+      <c r="E75" t="s">
+        <v>92</v>
+      </c>
+      <c r="F75" t="s">
+        <v>302</v>
+      </c>
+      <c r="G75" t="s">
+        <v>185</v>
+      </c>
+      <c r="H75" t="s">
+        <v>229</v>
+      </c>
+      <c r="I75" t="s">
+        <v>320</v>
+      </c>
+      <c r="J75" t="s">
+        <v>277</v>
+      </c>
+      <c r="K75" t="s">
+        <v>81</v>
+      </c>
+      <c r="L75" t="s">
+        <v>182</v>
+      </c>
+      <c r="M75" t="s">
+        <v>16</v>
+      </c>
+      <c r="N75" t="s">
+        <v>76</v>
+      </c>
+      <c r="O75" t="s">
+        <v>28</v>
+      </c>
+      <c r="P75" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>411</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" t="s">
+        <v>255</v>
+      </c>
+      <c r="D76" t="s">
+        <v>186</v>
+      </c>
+      <c r="E76" t="s">
+        <v>312</v>
+      </c>
+      <c r="F76" t="s">
+        <v>799</v>
+      </c>
+      <c r="G76" t="s">
+        <v>56</v>
+      </c>
+      <c r="H76" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76" t="s">
+        <v>800</v>
+      </c>
+      <c r="J76" t="s">
+        <v>188</v>
+      </c>
+      <c r="K76" t="s">
+        <v>36</v>
+      </c>
+      <c r="L76" t="s">
+        <v>760</v>
+      </c>
+      <c r="M76" t="s">
+        <v>798</v>
+      </c>
+      <c r="N76" t="s">
+        <v>314</v>
+      </c>
+      <c r="O76" t="s">
+        <v>801</v>
+      </c>
+      <c r="P76" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>413</v>
+      </c>
+      <c r="B77" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" t="s">
+        <v>144</v>
+      </c>
+      <c r="E77" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" t="s">
+        <v>803</v>
+      </c>
+      <c r="G77" t="s">
+        <v>251</v>
+      </c>
+      <c r="H77" t="s">
+        <v>79</v>
+      </c>
+      <c r="I77" t="s">
+        <v>701</v>
+      </c>
+      <c r="J77" t="s">
+        <v>738</v>
+      </c>
+      <c r="K77" t="s">
+        <v>81</v>
+      </c>
+      <c r="L77" t="s">
+        <v>117</v>
+      </c>
+      <c r="M77" t="s">
+        <v>358</v>
+      </c>
+      <c r="N77" t="s">
+        <v>247</v>
+      </c>
+      <c r="O77" t="s">
+        <v>637</v>
+      </c>
+      <c r="P77" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>414</v>
+      </c>
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
+        <v>59</v>
+      </c>
+      <c r="D78" t="s">
+        <v>397</v>
+      </c>
+      <c r="E78" t="s">
+        <v>289</v>
+      </c>
+      <c r="F78" t="s">
+        <v>192</v>
+      </c>
+      <c r="G78" t="s">
+        <v>237</v>
+      </c>
+      <c r="H78" t="s">
+        <v>253</v>
+      </c>
+      <c r="I78" t="s">
+        <v>729</v>
+      </c>
+      <c r="J78" t="s">
+        <v>155</v>
+      </c>
+      <c r="K78" t="s">
+        <v>39</v>
+      </c>
+      <c r="L78" t="s">
+        <v>91</v>
+      </c>
+      <c r="M78" t="s">
+        <v>20</v>
+      </c>
+      <c r="N78" t="s">
+        <v>257</v>
+      </c>
+      <c r="O78" t="s">
+        <v>216</v>
+      </c>
+      <c r="P78" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>643</v>
+      </c>
+      <c r="B79" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" t="s">
+        <v>29</v>
+      </c>
+      <c r="E79" t="s">
+        <v>139</v>
+      </c>
+      <c r="F79" t="s">
+        <v>75</v>
+      </c>
+      <c r="G79" t="s">
+        <v>241</v>
+      </c>
+      <c r="H79" t="s">
+        <v>96</v>
+      </c>
+      <c r="I79" t="s">
+        <v>101</v>
+      </c>
+      <c r="J79" t="s">
+        <v>101</v>
+      </c>
+      <c r="K79" t="s">
+        <v>81</v>
+      </c>
+      <c r="L79" t="s">
+        <v>93</v>
+      </c>
+      <c r="M79" t="s">
+        <v>387</v>
+      </c>
+      <c r="N79" t="s">
+        <v>89</v>
+      </c>
+      <c r="O79" t="s">
+        <v>249</v>
+      </c>
+      <c r="P79" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>415</v>
+      </c>
+      <c r="B80" t="s">
+        <v>39</v>
+      </c>
+      <c r="C80" t="s">
+        <v>250</v>
+      </c>
+      <c r="D80" t="s">
+        <v>267</v>
+      </c>
+      <c r="E80" t="s">
+        <v>172</v>
+      </c>
+      <c r="F80" t="s">
+        <v>804</v>
+      </c>
+      <c r="G80" t="s">
+        <v>768</v>
+      </c>
+      <c r="H80" t="s">
+        <v>175</v>
+      </c>
+      <c r="I80" t="s">
+        <v>244</v>
+      </c>
+      <c r="J80" t="s">
+        <v>735</v>
+      </c>
+      <c r="K80" t="s">
+        <v>39</v>
+      </c>
+      <c r="L80" t="s">
+        <v>303</v>
+      </c>
+      <c r="M80" t="s">
+        <v>122</v>
+      </c>
+      <c r="N80" t="s">
+        <v>37</v>
+      </c>
+      <c r="O80" t="s">
+        <v>669</v>
+      </c>
+      <c r="P80" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>418</v>
+      </c>
+      <c r="B81" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" t="s">
+        <v>90</v>
+      </c>
+      <c r="D81" t="s">
+        <v>76</v>
+      </c>
+      <c r="E81" t="s">
+        <v>96</v>
+      </c>
+      <c r="F81" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" t="s">
+        <v>85</v>
+      </c>
+      <c r="H81" t="s">
+        <v>40</v>
+      </c>
+      <c r="I81" t="s">
+        <v>247</v>
+      </c>
+      <c r="J81" t="s">
+        <v>78</v>
+      </c>
+      <c r="K81" t="s">
+        <v>81</v>
+      </c>
+      <c r="L81" t="s">
+        <v>93</v>
+      </c>
+      <c r="M81" t="s">
+        <v>387</v>
+      </c>
+      <c r="N81" t="s">
+        <v>241</v>
+      </c>
+      <c r="O81" t="s">
+        <v>631</v>
+      </c>
+      <c r="P81" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>419</v>
+      </c>
+      <c r="B82" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82" t="s">
+        <v>91</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" t="s">
+        <v>162</v>
+      </c>
+      <c r="F82" t="s">
+        <v>769</v>
+      </c>
+      <c r="G82" t="s">
+        <v>220</v>
+      </c>
+      <c r="H82" t="s">
+        <v>93</v>
+      </c>
+      <c r="I82" t="s">
+        <v>176</v>
+      </c>
+      <c r="J82" t="s">
+        <v>201</v>
+      </c>
+      <c r="K82" t="s">
+        <v>81</v>
+      </c>
+      <c r="L82" t="s">
+        <v>102</v>
+      </c>
+      <c r="M82" t="s">
+        <v>233</v>
+      </c>
+      <c r="N82" t="s">
+        <v>181</v>
+      </c>
+      <c r="O82" t="s">
+        <v>741</v>
+      </c>
+      <c r="P82" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>420</v>
+      </c>
+      <c r="B83" t="s">
+        <v>39</v>
+      </c>
+      <c r="C83" t="s">
+        <v>25</v>
+      </c>
+      <c r="D83" t="s">
+        <v>178</v>
+      </c>
+      <c r="E83" t="s">
+        <v>139</v>
+      </c>
+      <c r="F83" t="s">
+        <v>320</v>
+      </c>
+      <c r="G83" t="s">
+        <v>223</v>
+      </c>
+      <c r="H83" t="s">
+        <v>96</v>
+      </c>
+      <c r="I83" t="s">
+        <v>135</v>
+      </c>
+      <c r="J83" t="s">
+        <v>307</v>
+      </c>
+      <c r="K83" t="s">
+        <v>39</v>
+      </c>
+      <c r="L83" t="s">
+        <v>200</v>
+      </c>
+      <c r="M83" t="s">
+        <v>176</v>
+      </c>
+      <c r="N83" t="s">
+        <v>17</v>
+      </c>
+      <c r="O83" t="s">
+        <v>214</v>
+      </c>
+      <c r="P83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>421</v>
+      </c>
+      <c r="B84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C84" t="s">
+        <v>25</v>
+      </c>
+      <c r="D84" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" t="s">
+        <v>247</v>
+      </c>
+      <c r="F84" t="s">
+        <v>174</v>
+      </c>
+      <c r="G84" t="s">
+        <v>81</v>
+      </c>
+      <c r="H84" t="s">
+        <v>79</v>
+      </c>
+      <c r="I84" t="s">
+        <v>222</v>
+      </c>
+      <c r="J84" t="s">
+        <v>20</v>
+      </c>
+      <c r="K84" t="s">
+        <v>39</v>
+      </c>
+      <c r="L84" t="s">
+        <v>82</v>
+      </c>
+      <c r="M84" t="s">
+        <v>182</v>
+      </c>
+      <c r="N84" t="s">
+        <v>76</v>
+      </c>
+      <c r="O84" t="s">
+        <v>741</v>
+      </c>
+      <c r="P84" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>422</v>
+      </c>
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" t="s">
+        <v>116</v>
+      </c>
+      <c r="D85" t="s">
+        <v>287</v>
+      </c>
+      <c r="E85" t="s">
+        <v>118</v>
+      </c>
+      <c r="F85" t="s">
+        <v>252</v>
+      </c>
+      <c r="G85" t="s">
+        <v>309</v>
+      </c>
+      <c r="H85" t="s">
+        <v>51</v>
+      </c>
+      <c r="I85" t="s">
+        <v>691</v>
+      </c>
+      <c r="J85" t="s">
+        <v>776</v>
+      </c>
+      <c r="K85" t="s">
+        <v>180</v>
+      </c>
+      <c r="L85" t="s">
+        <v>680</v>
+      </c>
+      <c r="M85" t="s">
+        <v>742</v>
+      </c>
+      <c r="N85" t="s">
+        <v>765</v>
+      </c>
+      <c r="O85" t="s">
+        <v>805</v>
+      </c>
+      <c r="P85" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>424</v>
+      </c>
+      <c r="B86" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" t="s">
+        <v>16</v>
+      </c>
+      <c r="D86" t="s">
+        <v>17</v>
+      </c>
+      <c r="E86" t="s">
+        <v>213</v>
+      </c>
+      <c r="F86" t="s">
+        <v>176</v>
+      </c>
+      <c r="G86" t="s">
+        <v>42</v>
+      </c>
+      <c r="H86" t="s">
+        <v>213</v>
+      </c>
+      <c r="I86" t="s">
+        <v>222</v>
+      </c>
+      <c r="J86" t="s">
+        <v>38</v>
+      </c>
+      <c r="K86" t="s">
+        <v>36</v>
+      </c>
+      <c r="L86" t="s">
+        <v>131</v>
+      </c>
+      <c r="M86" t="s">
+        <v>193</v>
+      </c>
+      <c r="N86" t="s">
+        <v>161</v>
+      </c>
+      <c r="O86" t="s">
+        <v>148</v>
+      </c>
+      <c r="P86" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>425</v>
+      </c>
+      <c r="B87" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" t="s">
+        <v>86</v>
+      </c>
+      <c r="D87" t="s">
+        <v>29</v>
+      </c>
+      <c r="E87" t="s">
+        <v>289</v>
+      </c>
+      <c r="F87" t="s">
+        <v>666</v>
+      </c>
+      <c r="G87" t="s">
+        <v>31</v>
+      </c>
+      <c r="H87" t="s">
+        <v>253</v>
+      </c>
+      <c r="I87" t="s">
+        <v>666</v>
+      </c>
+      <c r="J87" t="s">
+        <v>31</v>
+      </c>
+      <c r="K87" t="s">
+        <v>39</v>
+      </c>
+      <c r="L87" t="s">
+        <v>82</v>
+      </c>
+      <c r="M87" t="s">
+        <v>182</v>
+      </c>
+      <c r="N87" t="s">
+        <v>257</v>
+      </c>
+      <c r="O87" t="s">
+        <v>258</v>
+      </c>
+      <c r="P87" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>644</v>
+      </c>
+      <c r="B88" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" t="s">
+        <v>45</v>
+      </c>
+      <c r="D88" t="s">
+        <v>191</v>
+      </c>
+      <c r="E88" t="s">
+        <v>213</v>
+      </c>
+      <c r="F88" t="s">
+        <v>807</v>
+      </c>
+      <c r="G88" t="s">
+        <v>20</v>
+      </c>
+      <c r="H88" t="s">
+        <v>213</v>
+      </c>
+      <c r="I88" t="s">
+        <v>154</v>
+      </c>
+      <c r="J88" t="s">
+        <v>238</v>
+      </c>
+      <c r="K88" t="s">
+        <v>36</v>
+      </c>
+      <c r="L88" t="s">
+        <v>200</v>
+      </c>
+      <c r="M88" t="s">
+        <v>128</v>
+      </c>
+      <c r="N88" t="s">
+        <v>161</v>
+      </c>
+      <c r="O88" t="s">
+        <v>48</v>
+      </c>
+      <c r="P88" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>426</v>
+      </c>
+      <c r="B89" t="s">
+        <v>39</v>
+      </c>
+      <c r="C89" t="s">
+        <v>171</v>
+      </c>
+      <c r="D89" t="s">
+        <v>22</v>
+      </c>
+      <c r="E89" t="s">
+        <v>151</v>
+      </c>
+      <c r="F89" t="s">
+        <v>633</v>
+      </c>
+      <c r="G89" t="s">
+        <v>232</v>
+      </c>
+      <c r="H89" t="s">
+        <v>153</v>
+      </c>
+      <c r="I89" t="s">
+        <v>45</v>
+      </c>
+      <c r="J89" t="s">
+        <v>217</v>
+      </c>
+      <c r="K89" t="s">
+        <v>36</v>
+      </c>
+      <c r="L89" t="s">
+        <v>200</v>
+      </c>
+      <c r="M89" t="s">
+        <v>128</v>
+      </c>
+      <c r="N89" t="s">
+        <v>207</v>
+      </c>
+      <c r="O89" t="s">
+        <v>729</v>
+      </c>
+      <c r="P89" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>427</v>
+      </c>
+      <c r="B90" t="s">
+        <v>39</v>
+      </c>
+      <c r="C90" t="s">
+        <v>90</v>
+      </c>
+      <c r="D90" t="s">
+        <v>76</v>
+      </c>
+      <c r="E90" t="s">
+        <v>139</v>
+      </c>
+      <c r="F90" t="s">
+        <v>72</v>
+      </c>
+      <c r="G90" t="s">
+        <v>750</v>
+      </c>
+      <c r="H90" t="s">
+        <v>96</v>
+      </c>
+      <c r="I90" t="s">
+        <v>106</v>
+      </c>
+      <c r="J90" t="s">
+        <v>72</v>
+      </c>
+      <c r="K90" t="s">
+        <v>39</v>
+      </c>
+      <c r="L90" t="s">
+        <v>93</v>
+      </c>
+      <c r="M90" t="s">
+        <v>177</v>
+      </c>
+      <c r="N90" t="s">
+        <v>17</v>
+      </c>
+      <c r="O90" t="s">
+        <v>72</v>
+      </c>
+      <c r="P90" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>428</v>
+      </c>
+      <c r="B91" t="s">
+        <v>39</v>
+      </c>
+      <c r="C91" t="s">
+        <v>197</v>
+      </c>
+      <c r="D91" t="s">
+        <v>729</v>
+      </c>
+      <c r="E91" t="s">
+        <v>123</v>
+      </c>
+      <c r="F91" t="s">
+        <v>752</v>
+      </c>
+      <c r="G91" t="s">
+        <v>633</v>
+      </c>
+      <c r="H91" t="s">
+        <v>126</v>
+      </c>
+      <c r="I91" t="s">
+        <v>778</v>
+      </c>
+      <c r="J91" t="s">
+        <v>264</v>
+      </c>
+      <c r="K91" t="s">
+        <v>105</v>
+      </c>
+      <c r="L91" t="s">
+        <v>303</v>
+      </c>
+      <c r="M91" t="s">
+        <v>733</v>
+      </c>
+      <c r="N91" t="s">
+        <v>18</v>
+      </c>
+      <c r="O91" t="s">
+        <v>197</v>
+      </c>
+      <c r="P91" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:P91" xr:uid="{E35F80F3-DC97-4223-AF5E-5C8A1EBDC247}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6683570-8DA7-420B-BFAB-3BB55B981681}">
   <dimension ref="A1:P91"/>
   <sheetViews>
@@ -16219,7 +21111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82987BA2-B919-43D2-BB30-4E483779E7E0}">
   <dimension ref="A1:P91"/>
   <sheetViews>

</xml_diff>